<commit_message>
added pages and test modules
</commit_message>
<xml_diff>
--- a/PytestAssignmentMain/TestData/MyNotesAppData.xlsx
+++ b/PytestAssignmentMain/TestData/MyNotesAppData.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priyankverma\PycharmProjects\PytestAssignmentMain\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B06B99C-6D73-4CBE-A1D0-A5659537CBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9E1619-2CF3-44DB-8B06-ACF46284339C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D6283F87-734C-429D-B6B1-D359DC557368}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{D6283F87-734C-429D-B6B1-D359DC557368}"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
     <sheet name="LoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="UpdateProfileData" sheetId="4" r:id="rId3"/>
+    <sheet name="ChangePasswordData" sheetId="5" r:id="rId4"/>
+    <sheet name="AddNoteForHome" sheetId="6" r:id="rId5"/>
+    <sheet name="AddNoteForWork" sheetId="7" r:id="rId6"/>
+    <sheet name="AddNoteForPersonal" sheetId="8" r:id="rId7"/>
+    <sheet name="EditNoteForHome" sheetId="9" r:id="rId8"/>
+    <sheet name="EditNoteForWork" sheetId="10" r:id="rId9"/>
+    <sheet name="EditNoteForPersonal" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>email</t>
   </si>
@@ -73,6 +81,81 @@
   </si>
   <si>
     <t>https://practice.expandtesting.com/notes/app</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>9625181982</t>
+  </si>
+  <si>
+    <t>Profile updated successful</t>
+  </si>
+  <si>
+    <t>alertMessage</t>
+  </si>
+  <si>
+    <t>The password was successfully updated</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Clothes, Groceries, Furnitures</t>
+  </si>
+  <si>
+    <t>Main Assignment</t>
+  </si>
+  <si>
+    <t>Build Framework, Write Test Cases, Generate Report</t>
+  </si>
+  <si>
+    <t>Workout</t>
+  </si>
+  <si>
+    <t>Chest Training, Triceps Training, Legs Training</t>
+  </si>
+  <si>
+    <t>Deloitte-USI</t>
+  </si>
+  <si>
+    <t>Read Novel</t>
+  </si>
+  <si>
+    <t>Read the novel 'Rich Dad Poor Dad'.</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Manual Testing, Automation Testing, Functional &amp; Non-functional Testing.</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>Bedroom, Drawing room, Hall, and Kitchen.</t>
   </si>
 </sst>
 </file>
@@ -104,12 +187,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,10 +214,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -447,7 +537,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,19 +546,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -499,12 +589,47 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5E5C04-983B-49D7-A778-1A4F76DBD96A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="50.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2871921C-AFC9-4748-A759-D17467058AE6}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,13 +639,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -543,4 +668,287 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2D0B30-F99E-4169-9BA9-20355813E923}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="30.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E51EDB-5497-4906-8BC9-54F7C725FA84}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" customWidth="1"/>
+    <col min="4" max="4" width="30.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6E7BAE06-14F3-4A00-A12C-A17D1C7670E4}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{33CAE9C5-100B-4BA8-93D9-4F3C56B3BDA4}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{C3766AB0-9B94-4534-ADFB-5926510BC014}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{F85A9951-6895-4B2C-95D6-215E85CC4E7A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D6E7A1-0BEB-425B-9B76-5C74A51687B4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="50.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298563D9-BE22-49A0-8BA8-B306EAE17814}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="50.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D20505-AAA6-4E51-869A-35EDD2AE3A41}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="50.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5AF5A6-2A76-47AB-A26C-E7C376A34AB5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="50.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7493EF41-E9FE-45CE-88CB-033699144791}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="50.6328125" customWidth="1"/>
+    <col min="2" max="2" width="64.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
logs and report added
</commit_message>
<xml_diff>
--- a/PytestAssignmentMain/TestData/MyNotesAppData.xlsx
+++ b/PytestAssignmentMain/TestData/MyNotesAppData.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priyankverma\PycharmProjects\PytestAssignmentMain\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9E1619-2CF3-44DB-8B06-ACF46284339C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB77299A-625D-4648-B4BA-499D0D60EC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{D6283F87-734C-429D-B6B1-D359DC557368}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{D6283F87-734C-429D-B6B1-D359DC557368}"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
     <sheet name="LoginData" sheetId="2" r:id="rId2"/>
     <sheet name="UpdateProfileData" sheetId="4" r:id="rId3"/>
-    <sheet name="ChangePasswordData" sheetId="5" r:id="rId4"/>
+    <sheet name="ChangePasswordData" sheetId="12" r:id="rId4"/>
     <sheet name="AddNoteForHome" sheetId="6" r:id="rId5"/>
     <sheet name="AddNoteForWork" sheetId="7" r:id="rId6"/>
     <sheet name="AddNoteForPersonal" sheetId="8" r:id="rId7"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>email</t>
   </si>
@@ -59,103 +59,118 @@
     <t>successAlert</t>
   </si>
   <si>
+    <t>Pass@123</t>
+  </si>
+  <si>
+    <t>User account created successfully</t>
+  </si>
+  <si>
+    <t>An account already exists with the same email address</t>
+  </si>
+  <si>
+    <t>failedAlert</t>
+  </si>
+  <si>
+    <t>currentUrl</t>
+  </si>
+  <si>
+    <t>https://practice.expandtesting.com/notes/app</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>9625181982</t>
+  </si>
+  <si>
+    <t>Profile updated successful</t>
+  </si>
+  <si>
+    <t>alertMessage</t>
+  </si>
+  <si>
+    <t>The password was successfully updated</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Clothes, Groceries, Furnitures</t>
+  </si>
+  <si>
+    <t>Main Assignment</t>
+  </si>
+  <si>
+    <t>Build Framework, Write Test Cases, Generate Report</t>
+  </si>
+  <si>
+    <t>Workout</t>
+  </si>
+  <si>
+    <t>Chest Training, Triceps Training, Legs Training</t>
+  </si>
+  <si>
+    <t>Deloitte-USI</t>
+  </si>
+  <si>
+    <t>Read Novel</t>
+  </si>
+  <si>
+    <t>Read the novel 'Rich Dad Poor Dad'.</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Manual Testing, Automation Testing, Functional &amp; Non-functional Testing.</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>Bedroom, Drawing room, Hall, and Kitchen.</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>Microsoft-USI</t>
+  </si>
+  <si>
+    <t>Shantanu Verma</t>
+  </si>
+  <si>
+    <t>Shashank Sharma</t>
+  </si>
+  <si>
+    <t>johnwilliams@gmail.com</t>
+  </si>
+  <si>
+    <t>John Williams</t>
+  </si>
+  <si>
     <t>priyankverma@deloitte.com</t>
-  </si>
-  <si>
-    <t>Priyank Verma</t>
-  </si>
-  <si>
-    <t>Pass@123</t>
-  </si>
-  <si>
-    <t>User account created successfully</t>
-  </si>
-  <si>
-    <t>An account already exists with the same email address</t>
-  </si>
-  <si>
-    <t>failedAlert</t>
-  </si>
-  <si>
-    <t>currentUrl</t>
-  </si>
-  <si>
-    <t>https://practice.expandtesting.com/notes/app</t>
-  </si>
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
-    <t>companyName</t>
-  </si>
-  <si>
-    <t>fullName</t>
-  </si>
-  <si>
-    <t>9625181982</t>
-  </si>
-  <si>
-    <t>Profile updated successful</t>
-  </si>
-  <si>
-    <t>alertMessage</t>
-  </si>
-  <si>
-    <t>The password was successfully updated</t>
-  </si>
-  <si>
-    <t>currentPassword</t>
-  </si>
-  <si>
-    <t>newPassword</t>
-  </si>
-  <si>
-    <t>Password@123</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Shopping</t>
-  </si>
-  <si>
-    <t>Clothes, Groceries, Furnitures</t>
-  </si>
-  <si>
-    <t>Main Assignment</t>
-  </si>
-  <si>
-    <t>Build Framework, Write Test Cases, Generate Report</t>
-  </si>
-  <si>
-    <t>Workout</t>
-  </si>
-  <si>
-    <t>Chest Training, Triceps Training, Legs Training</t>
-  </si>
-  <si>
-    <t>Deloitte-USI</t>
-  </si>
-  <si>
-    <t>Read Novel</t>
-  </si>
-  <si>
-    <t>Read the novel 'Rich Dad Poor Dad'.</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Manual Testing, Automation Testing, Functional &amp; Non-functional Testing.</t>
-  </si>
-  <si>
-    <t>Painting</t>
-  </si>
-  <si>
-    <t>Bedroom, Drawing room, Hall, and Kitchen.</t>
   </si>
 </sst>
 </file>
@@ -537,7 +552,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,24 +574,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -604,18 +619,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -629,7 +644,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,24 +661,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3C328AA9-6C7D-47E1-9EA6-3033FE87EAE3}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{629CA096-658F-4722-94A0-9DDB8B9750C2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{629CA096-658F-4722-94A0-9DDB8B9750C2}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{B6DCB687-85F3-4DD7-8A25-7EDAB689132D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -672,10 +687,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2D0B30-F99E-4169-9BA9-20355813E923}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,30 +700,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -718,62 +747,47 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E51EDB-5497-4906-8BC9-54F7C725FA84}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B061B7EE-13F5-4A4B-B83D-E075BB046275}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="34.54296875" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" customWidth="1"/>
+    <col min="1" max="3" width="50.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6E7BAE06-14F3-4A00-A12C-A17D1C7670E4}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{33CAE9C5-100B-4BA8-93D9-4F3C56B3BDA4}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{C3766AB0-9B94-4534-ADFB-5926510BC014}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{F85A9951-6895-4B2C-95D6-215E85CC4E7A}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{058FB484-585E-46B9-AE6E-5D54EC2FD66E}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{3A5E2C75-E9A4-4D0F-B734-FB4F8D29AA0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -782,7 +796,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,18 +806,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -827,18 +841,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +866,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,18 +876,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -886,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5AF5A6-2A76-47AB-A26C-E7C376A34AB5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -897,18 +911,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -933,18 +947,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>